<commit_message>
Fix parser for notes, update readme & build project
</commit_message>
<xml_diff>
--- a/excel/brief_example_with_notes.xlsx
+++ b/excel/brief_example_with_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZhernokE\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE3A4DA-D11B-4211-96CB-C5B8B798FA5E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290022E8-C1C6-4CD2-98FE-659026664C9A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="601" xr2:uid="{D56199A6-23DC-9C48-9AED-27640EB21542}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>FSC</t>
   </si>
@@ -157,15 +157,6 @@
     <t>Цена 1 шт. без спец предложения 230 р</t>
   </si>
   <si>
-    <t>*</t>
-  </si>
-  <si>
-    <t>**</t>
-  </si>
-  <si>
-    <t>***</t>
-  </si>
-  <si>
     <t>Украшение на шею "Либби"</t>
   </si>
   <si>
@@ -179,9 +170,6 @@
   </si>
   <si>
     <t xml:space="preserve"> аметист</t>
-  </si>
-  <si>
-    <t>****</t>
   </si>
   <si>
     <t>Цена 1 шт. без спец предложения 430 р</t>
@@ -691,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBE2B86-7C91-E04C-83EE-E98EF11EDA0F}">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
@@ -844,8 +832,8 @@
       <c r="K6" s="18">
         <v>139</v>
       </c>
-      <c r="L6" t="s">
-        <v>41</v>
+      <c r="L6">
+        <v>1</v>
       </c>
       <c r="M6" t="s">
         <v>32</v>
@@ -876,8 +864,8 @@
       <c r="K7" s="9">
         <v>179</v>
       </c>
-      <c r="L7" t="s">
-        <v>41</v>
+      <c r="L7">
+        <v>1</v>
       </c>
       <c r="M7" t="s">
         <v>24</v>
@@ -908,8 +896,8 @@
       <c r="K8" s="9">
         <v>169</v>
       </c>
-      <c r="L8" t="s">
-        <v>42</v>
+      <c r="L8">
+        <v>2</v>
       </c>
       <c r="M8" t="s">
         <v>24</v>
@@ -939,8 +927,8 @@
       <c r="K9" s="9">
         <v>149</v>
       </c>
-      <c r="L9" t="s">
-        <v>42</v>
+      <c r="L9">
+        <v>2</v>
       </c>
       <c r="M9" t="s">
         <v>24</v>
@@ -970,8 +958,8 @@
       <c r="K10" s="9">
         <v>179</v>
       </c>
-      <c r="L10" t="s">
-        <v>43</v>
+      <c r="L10">
+        <v>3</v>
       </c>
       <c r="M10" t="s">
         <v>24</v>
@@ -989,28 +977,28 @@
         <v>987654</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="K11" s="1">
         <v>550</v>
       </c>
-      <c r="L11" t="s">
-        <v>49</v>
+      <c r="L11">
+        <v>4</v>
       </c>
       <c r="M11" t="s">
         <v>24</v>
       </c>
       <c r="P11" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="47.25">
@@ -1021,33 +1009,33 @@
         <v>987654</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="K12" s="1">
         <v>550</v>
       </c>
-      <c r="L12" t="s">
-        <v>49</v>
+      <c r="L12">
+        <v>4</v>
       </c>
       <c r="M12" t="s">
         <v>24</v>
       </c>
       <c r="P12" s="9" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:17" s="13" customFormat="1">
       <c r="A13" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D13" s="14"/>
     </row>
@@ -1096,8 +1084,8 @@
       <c r="K15" s="1">
         <v>499</v>
       </c>
-      <c r="L15" t="s">
-        <v>41</v>
+      <c r="L15">
+        <v>1</v>
       </c>
       <c r="M15" t="s">
         <v>29</v>
@@ -1141,22 +1129,22 @@
         <v>123789</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="K17" s="1">
         <v>400</v>
       </c>
-      <c r="L17" t="s">
-        <v>41</v>
+      <c r="L17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12">
@@ -1167,22 +1155,22 @@
         <v>123789</v>
       </c>
       <c r="D18" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" t="s">
+        <v>49</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="K18" s="1">
         <v>400</v>
       </c>
-      <c r="L18" t="s">
-        <v>41</v>
+      <c r="L18">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>